<commit_message>
Atualização do form de lançamentos diários
</commit_message>
<xml_diff>
--- a/crono.xlsx
+++ b/crono.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,8 +474,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>45519</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>15/08/2024</t>
+        </is>
       </c>
       <c r="C2" t="n">
         <v>2068352</v>
@@ -508,8 +506,10 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>45519</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>15/08/2024</t>
+        </is>
       </c>
       <c r="C3" t="n">
         <v>2068352</v>
@@ -517,7 +517,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SACOS PARA HAMBURGÃO</t>
+          <t>SACOS PARA HOT DOG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -538,8 +538,10 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>45519</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>15/08/2024</t>
+        </is>
       </c>
       <c r="C4" t="n">
         <v>2068352</v>
@@ -547,7 +549,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>SACOS PARA HOT DOG</t>
+          <t>SACOS PARA HAMBURGÃO</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -568,8 +570,10 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>45519</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>15/08/2024</t>
+        </is>
       </c>
       <c r="C5" t="n">
         <v>2068353</v>
@@ -598,8 +602,10 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>45519</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>15/08/2024</t>
+        </is>
       </c>
       <c r="C6" t="n">
         <v>2068351</v>
@@ -621,6 +627,390 @@
         </is>
       </c>
       <c r="H6" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2068354</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LUVAS PLÁSTICAS</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BOMPACK</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>100Un.</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2068354</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>PAPEL MANTEIGA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BOMPACK</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4m</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2068354</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>PAPEL ALUMINIO</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BOMPACK</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>4m</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2068358</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>SACOS PLÁSTICOS</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BOT</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>20Un.</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2068358</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>SACOS PARA LIXO</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>BOM</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>5Un.</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2068358</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>SACOS PLÁSTICOS P/ ALIMENTOS</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>BOT</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>50Un.</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2068361</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>SACOS PARA LIXO</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>BOM</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>50Un.</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2068361</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>SACOS PARA LIXO</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>BOT</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>10Un.</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2068361</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>SACOS PARA LIXO</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>BOT</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>10Un.</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2068362</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SACOS PARA LIXO</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>BOT</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>4Un.</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2068363</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SACOS PARA LIXO</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>FAM ROLL</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>30Un.</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2068363</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>SACOS PARA LIXO</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>FAM ROLL</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>30Un.</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
         <v>13</v>
       </c>
     </row>

</xml_diff>